<commit_message>
More understandable excel file output
</commit_message>
<xml_diff>
--- a/differences.xlsx
+++ b/differences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hervas Brothers\Documents\ClearCO2\CO2_matching_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D27FD0E7-C6EE-4A80-B24E-084FAE1C1CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A736E1F-FFDB-4B17-90FC-811B6F7AB398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
   <si>
     <t>Matched Subcategory</t>
   </si>
@@ -116,6 +116,159 @@
   </si>
   <si>
     <t>Other non-ferrous metal products</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Grains and grain-based products</t>
+  </si>
+  <si>
+    <t>Cereals and cereal primary derivatives</t>
+  </si>
+  <si>
+    <t>Cereal grains (and cereal-like grains)</t>
+  </si>
+  <si>
+    <t>Mixture of grains</t>
+  </si>
+  <si>
+    <t>Barley and similar-</t>
+  </si>
+  <si>
+    <t>Barley grains</t>
+  </si>
+  <si>
+    <t>Barley grain, pearled</t>
+  </si>
+  <si>
+    <t>Buckwheat and other pseudo-cereals and similar-</t>
+  </si>
+  <si>
+    <t>Buckwheat</t>
+  </si>
+  <si>
+    <t>Amaranth grains</t>
+  </si>
+  <si>
+    <t>Foxtail amaranth grain</t>
+  </si>
+  <si>
+    <t>Red amaranth grains</t>
+  </si>
+  <si>
+    <t>Prince of Wales-feather amaranth grain</t>
+  </si>
+  <si>
+    <t>Kaniwa grain</t>
+  </si>
+  <si>
+    <t>Quinoa grain</t>
+  </si>
+  <si>
+    <t>Maize and similar-</t>
+  </si>
+  <si>
+    <t>Popcorn kernels</t>
+  </si>
+  <si>
+    <t>Teosinte grain</t>
+  </si>
+  <si>
+    <t>Maize grain</t>
+  </si>
+  <si>
+    <t>Indian corn grain</t>
+  </si>
+  <si>
+    <t>Common millet and similar-</t>
+  </si>
+  <si>
+    <t>Common millet grain</t>
+  </si>
+  <si>
+    <t>Black fonio grain</t>
+  </si>
+  <si>
+    <t>Canary grass grain</t>
+  </si>
+  <si>
+    <t>Finger millet grain</t>
+  </si>
+  <si>
+    <t>African millet grain</t>
+  </si>
+  <si>
+    <t>Foxtail millet grain</t>
+  </si>
+  <si>
+    <t>Job's tears grain</t>
+  </si>
+  <si>
+    <t>Little millet grain</t>
+  </si>
+  <si>
+    <t>Pearl millet grain</t>
+  </si>
+  <si>
+    <t>Teff grain</t>
+  </si>
+  <si>
+    <t>White fonio grain</t>
+  </si>
+  <si>
+    <t>Barnyard millet</t>
+  </si>
+  <si>
+    <t>Oat and similar-</t>
+  </si>
+  <si>
+    <t>Oat grain</t>
+  </si>
+  <si>
+    <t>Oat grain, red</t>
+  </si>
+  <si>
+    <t>Rice and similar-</t>
+  </si>
+  <si>
+    <t>Rice grain</t>
+  </si>
+  <si>
+    <t>Rice grain, brown</t>
+  </si>
+  <si>
+    <t>Rice grain, long-grain</t>
+  </si>
+  <si>
+    <t>Rice grain, mixed</t>
+  </si>
+  <si>
+    <t>Rice grain, red</t>
+  </si>
+  <si>
+    <t>Rice grain, polished</t>
+  </si>
+  <si>
+    <t>Rice grain, parboiled</t>
+  </si>
+  <si>
+    <t>Rice grain, glutinous</t>
+  </si>
+  <si>
+    <t>African rice grain</t>
+  </si>
+  <si>
+    <t>Hybrid Nerica®</t>
+  </si>
+  <si>
+    <t>Indian rice grain</t>
+  </si>
+  <si>
+    <t>Rye and similar-</t>
+  </si>
+  <si>
+    <t>Rye grain</t>
   </si>
 </sst>
 </file>
@@ -136,12 +289,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -171,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -179,6 +338,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -493,9 +654,10 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.53125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -505,8 +667,11 @@
         <v>1</v>
       </c>
       <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -520,25 +685,36 @@
       <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -548,8 +724,11 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -562,11 +741,14 @@
       <c r="D6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>9</v>
       </c>
@@ -579,11 +761,14 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>11</v>
       </c>
@@ -593,14 +778,17 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>12</v>
       </c>
@@ -613,11 +801,14 @@
       <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G9" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>13</v>
       </c>
@@ -627,14 +818,17 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>14</v>
       </c>
@@ -644,8 +838,11 @@
       <c r="C11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>20</v>
       </c>
@@ -661,8 +858,11 @@
       <c r="E12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>22</v>
       </c>
@@ -675,11 +875,14 @@
       <c r="D13" t="s">
         <v>23</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>23</v>
       </c>
@@ -689,14 +892,17 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>25</v>
       </c>
@@ -706,14 +912,17 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>27</v>
       </c>
@@ -729,8 +938,11 @@
       <c r="E16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>30</v>
       </c>
@@ -746,8 +958,11 @@
       <c r="E17" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>39</v>
       </c>
@@ -763,8 +978,11 @@
       <c r="E18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>44</v>
       </c>
@@ -780,8 +998,11 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>46</v>
       </c>
@@ -796,6 +1017,176 @@
       </c>
       <c r="E20" t="s">
         <v>23</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="G23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="G24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="G25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G30" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G40" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G45" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.45">
+      <c r="G51" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>